<commit_message>
Fix bugs in `Lab2`.
</commit_message>
<xml_diff>
--- a/Lab2/Solutions/Images/CreateT3Image.xlsx
+++ b/Lab2/Solutions/Images/CreateT3Image.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\UU_CS\Period2\1DL590\Lab2\Solutions\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC11D810-AC41-4167-87DC-D62855D44990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6668EDC9-5435-419C-A0BF-E3B75467C251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27250" yWindow="-3340" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="range_0_to_7" sheetId="2" r:id="rId1"/>
     <sheet name="range_0_to_1023" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -240,22 +242,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>16005.922602000001</c:v>
+                  <c:v>31361.158050999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5800.7288420000004</c:v>
+                  <c:v>21793.743456</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2241.9002919999998</c:v>
+                  <c:v>18201.669559000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1231.9810130000001</c:v>
+                  <c:v>18395.182689000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>633.09293400000001</c:v>
+                  <c:v>18223.721625999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>306.05244500000003</c:v>
+                  <c:v>19026.033731</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -319,22 +321,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3815.921081</c:v>
+                  <c:v>7919.3246589999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1449.3323330000001</c:v>
+                  <c:v>7164.2088810000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>710.2591480000001</c:v>
+                  <c:v>5689.1358129999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>993.95588800000007</c:v>
+                  <c:v>17202.302087</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>480.38099699999998</c:v>
+                  <c:v>15475.009431</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>237.699355</c:v>
+                  <c:v>14408.001976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -398,22 +400,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7701.0151599999999</c:v>
+                  <c:v>15770.135167999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2771.548816</c:v>
+                  <c:v>12107.079559</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1258.0418559999998</c:v>
+                  <c:v>10021.444551999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>915.01013999999998</c:v>
+                  <c:v>14937.551917999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>424.32018099999999</c:v>
+                  <c:v>13420.573001000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>212.49391900000001</c:v>
+                  <c:v>13786.35007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -981,22 +983,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>17655.989931</c:v>
+                  <c:v>51409.919654999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7209.8668660000003</c:v>
+                  <c:v>39009.161001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2555.6231209999996</c:v>
+                  <c:v>22195.226043999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1355.1126429999999</c:v>
+                  <c:v>21458.390769000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>680.70266700000002</c:v>
+                  <c:v>20856.703845</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>340.255718</c:v>
+                  <c:v>20898.758034999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1060,22 +1062,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5725.0118750000001</c:v>
+                  <c:v>12869.437148999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2232.1133879999998</c:v>
+                  <c:v>8415.3477679999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1026.3611820000001</c:v>
+                  <c:v>7642.031223</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1005.260578</c:v>
+                  <c:v>16479.643085</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>495.22111999999998</c:v>
+                  <c:v>15977.169236</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>242.75527299999999</c:v>
+                  <c:v>15971.148160000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1139,22 +1141,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7760.4177070000005</c:v>
+                  <c:v>14702.205522</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2599.9884700000002</c:v>
+                  <c:v>9982.4094800000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1229.5890260000001</c:v>
+                  <c:v>9433.6407829999989</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1101.5483589999999</c:v>
+                  <c:v>18330.801868000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>561.54473899999994</c:v>
+                  <c:v>17023.71298</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>282.53824599999996</c:v>
+                  <c:v>17170.486681000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1726,22 +1728,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>18054.149914999998</c:v>
+                  <c:v>35605.599368000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7039.8678739999996</c:v>
+                  <c:v>29850.519802000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3030.9825770000002</c:v>
+                  <c:v>22840.501103999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1522.8927490000001</c:v>
+                  <c:v>23151.701236000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>766.51370999999995</c:v>
+                  <c:v>23153.458517999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>371.91076600000002</c:v>
+                  <c:v>22764.920905000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1805,22 +1807,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10857.746391000001</c:v>
+                  <c:v>28544.136761999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4177.8266519999997</c:v>
+                  <c:v>19841.074765000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1723.855419</c:v>
+                  <c:v>13525.235440999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>987.9422780000001</c:v>
+                  <c:v>15802.498160000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>517.47326499999997</c:v>
+                  <c:v>16320.735236</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>256.23837800000001</c:v>
+                  <c:v>16129.511279999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1884,22 +1886,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>8544.1630320000004</c:v>
+                  <c:v>15693.545309000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2477.1184349999999</c:v>
+                  <c:v>8916.3725489999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1185.297722</c:v>
+                  <c:v>8550.9542799999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1691.6554269999999</c:v>
+                  <c:v>24738.169085999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>773.47422800000004</c:v>
+                  <c:v>24001.121573</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>395.77799499999998</c:v>
+                  <c:v>24267.876910999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2467,22 +2469,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>919.62301300000001</c:v>
+                  <c:v>1842.328088</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>417.60313600000001</c:v>
+                  <c:v>1630.8040209999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200.74024400000002</c:v>
+                  <c:v>1657.2839739999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.146281000000002</c:v>
+                  <c:v>1587.382398</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.621006000000001</c:v>
+                  <c:v>1557.1203330000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.334616</c:v>
+                  <c:v>1568.475103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2546,22 +2548,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>179.101314</c:v>
+                  <c:v>336.98767900000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156.03995900000001</c:v>
+                  <c:v>1289.4868859999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>116.41900199999999</c:v>
+                  <c:v>913.99323800000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88.838847999999999</c:v>
+                  <c:v>1391.7510339999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.236562000000003</c:v>
+                  <c:v>654.48222699999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.412404</c:v>
+                  <c:v>824.597082</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2625,22 +2627,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>696.66354899999999</c:v>
+                  <c:v>1338.4766599999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>585.83232200000009</c:v>
+                  <c:v>2214.1490180000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>535.49387899999999</c:v>
+                  <c:v>3685.9497850000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>338.45861099999996</c:v>
+                  <c:v>6352.0652230000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>218.7397</c:v>
+                  <c:v>6953.0150679999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>113.20912799999999</c:v>
+                  <c:v>8305.270579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3208,22 +3210,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1574.480401</c:v>
+                  <c:v>3143.5526620000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>705.70083900000009</c:v>
+                  <c:v>2792.2023709999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>279.65802000000002</c:v>
+                  <c:v>2534.4221979999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>164.550059</c:v>
+                  <c:v>2679.5521589999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81.694020000000009</c:v>
+                  <c:v>2646.4874009999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.356572999999997</c:v>
+                  <c:v>2602.847863</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3287,22 +3289,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>273.08965500000005</c:v>
+                  <c:v>516.59814600000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>246.65773300000001</c:v>
+                  <c:v>938.75314700000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>188.79276999999999</c:v>
+                  <c:v>1378.6770940000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>140.353972</c:v>
+                  <c:v>2314.187336</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.471094999999998</c:v>
+                  <c:v>1091.683689</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.931922999999998</c:v>
+                  <c:v>1419.085041</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3366,22 +3368,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1196.398173</c:v>
+                  <c:v>2345.0947659999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>738.58021900000006</c:v>
+                  <c:v>3015.3703369999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>648.26373999999998</c:v>
+                  <c:v>5437.6859489999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>424.941509</c:v>
+                  <c:v>7199.2589280000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>214.538827</c:v>
+                  <c:v>6590.7346710000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>108.432823</c:v>
+                  <c:v>6351.2031569999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3955,22 +3957,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1799.0464119999999</c:v>
+                  <c:v>3625.124945</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>771.92786100000001</c:v>
+                  <c:v>3370.6834079999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>365.542778</c:v>
+                  <c:v>2945.1253860000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>199.91519699999998</c:v>
+                  <c:v>3198.058125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.528789999999987</c:v>
+                  <c:v>3102.866888</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46.391167000000003</c:v>
+                  <c:v>2957.5107239999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4034,22 +4036,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>356.02531699999997</c:v>
+                  <c:v>697.07932600000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>298.03088600000001</c:v>
+                  <c:v>1434.622519</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>260.77903400000002</c:v>
+                  <c:v>1912.528129</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.761234999999999</c:v>
+                  <c:v>945.72881900000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.887888</c:v>
+                  <c:v>826.375765</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.647536000000001</c:v>
+                  <c:v>946.37794299999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4113,22 +4115,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1969.667256</c:v>
+                  <c:v>5328.0488609999993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1631.2498999999998</c:v>
+                  <c:v>8573.2238010000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1878.9681029999999</c:v>
+                  <c:v>9069.4713530000008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>945.63276300000007</c:v>
+                  <c:v>17577.511300999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>439.91199900000004</c:v>
+                  <c:v>15351.100666999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>228.96158499999999</c:v>
+                  <c:v>15542.536341000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8339,8 +8341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D48DDB0-D93D-443B-93BC-8B4B95643737}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X42" sqref="X42"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8378,13 +8380,13 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>16005.922602000001</v>
+        <v>31361.158050999999</v>
       </c>
       <c r="D2">
-        <v>3815.921081</v>
+        <v>7919.3246589999999</v>
       </c>
       <c r="E2">
-        <v>7701.0151599999999</v>
+        <v>15770.135167999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -8392,13 +8394,13 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>5800.7288420000004</v>
+        <v>21793.743456</v>
       </c>
       <c r="D3">
-        <v>1449.3323330000001</v>
+        <v>7164.2088810000005</v>
       </c>
       <c r="E3">
-        <v>2771.548816</v>
+        <v>12107.079559</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -8406,13 +8408,13 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>2241.9002919999998</v>
+        <v>18201.669559000002</v>
       </c>
       <c r="D4">
-        <v>710.2591480000001</v>
+        <v>5689.1358129999999</v>
       </c>
       <c r="E4">
-        <v>1258.0418559999998</v>
+        <v>10021.444551999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -8420,13 +8422,13 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>1231.9810130000001</v>
+        <v>18395.182689000001</v>
       </c>
       <c r="D5">
-        <v>993.95588800000007</v>
+        <v>17202.302087</v>
       </c>
       <c r="E5">
-        <v>915.01013999999998</v>
+        <v>14937.551917999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -8434,13 +8436,13 @@
         <v>32</v>
       </c>
       <c r="C6">
-        <v>633.09293400000001</v>
+        <v>18223.721625999999</v>
       </c>
       <c r="D6">
-        <v>480.38099699999998</v>
+        <v>15475.009431</v>
       </c>
       <c r="E6">
-        <v>424.32018099999999</v>
+        <v>13420.573001000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -8448,13 +8450,13 @@
         <v>64</v>
       </c>
       <c r="C7">
-        <v>306.05244500000003</v>
+        <v>19026.033731</v>
       </c>
       <c r="D7">
-        <v>237.699355</v>
+        <v>14408.001976</v>
       </c>
       <c r="E7">
-        <v>212.49391900000001</v>
+        <v>13786.35007</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -8465,13 +8467,13 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>17655.989931</v>
+        <v>51409.919654999998</v>
       </c>
       <c r="D8">
-        <v>5725.0118750000001</v>
+        <v>12869.437148999999</v>
       </c>
       <c r="E8">
-        <v>7760.4177070000005</v>
+        <v>14702.205522</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -8479,13 +8481,13 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>7209.8668660000003</v>
+        <v>39009.161001</v>
       </c>
       <c r="D9">
-        <v>2232.1133879999998</v>
+        <v>8415.3477679999996</v>
       </c>
       <c r="E9">
-        <v>2599.9884700000002</v>
+        <v>9982.4094800000003</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -8493,13 +8495,13 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>2555.6231209999996</v>
+        <v>22195.226043999999</v>
       </c>
       <c r="D10">
-        <v>1026.3611820000001</v>
+        <v>7642.031223</v>
       </c>
       <c r="E10">
-        <v>1229.5890260000001</v>
+        <v>9433.6407829999989</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
@@ -8507,13 +8509,13 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>1355.1126429999999</v>
+        <v>21458.390769000001</v>
       </c>
       <c r="D11">
-        <v>1005.260578</v>
+        <v>16479.643085</v>
       </c>
       <c r="E11">
-        <v>1101.5483589999999</v>
+        <v>18330.801868000002</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -8521,13 +8523,13 @@
         <v>32</v>
       </c>
       <c r="C12">
-        <v>680.70266700000002</v>
+        <v>20856.703845</v>
       </c>
       <c r="D12">
-        <v>495.22111999999998</v>
+        <v>15977.169236</v>
       </c>
       <c r="E12">
-        <v>561.54473899999994</v>
+        <v>17023.71298</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -8535,13 +8537,13 @@
         <v>64</v>
       </c>
       <c r="C13">
-        <v>340.255718</v>
+        <v>20898.758034999999</v>
       </c>
       <c r="D13">
-        <v>242.75527299999999</v>
+        <v>15971.148160000001</v>
       </c>
       <c r="E13">
-        <v>282.53824599999996</v>
+        <v>17170.486681000002</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -8552,13 +8554,13 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>18054.149914999998</v>
+        <v>35605.599368000003</v>
       </c>
       <c r="D14">
-        <v>10857.746391000001</v>
+        <v>28544.136761999998</v>
       </c>
       <c r="E14">
-        <v>8544.1630320000004</v>
+        <v>15693.545309000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -8566,13 +8568,13 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>7039.8678739999996</v>
+        <v>29850.519802000003</v>
       </c>
       <c r="D15">
-        <v>4177.8266519999997</v>
+        <v>19841.074765000001</v>
       </c>
       <c r="E15">
-        <v>2477.1184349999999</v>
+        <v>8916.3725489999997</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -8580,13 +8582,13 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>3030.9825770000002</v>
+        <v>22840.501103999999</v>
       </c>
       <c r="D16">
-        <v>1723.855419</v>
+        <v>13525.235440999999</v>
       </c>
       <c r="E16">
-        <v>1185.297722</v>
+        <v>8550.9542799999999</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.45">
@@ -8594,13 +8596,13 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>1522.8927490000001</v>
+        <v>23151.701236000001</v>
       </c>
       <c r="D17">
-        <v>987.9422780000001</v>
+        <v>15802.498160000001</v>
       </c>
       <c r="E17">
-        <v>1691.6554269999999</v>
+        <v>24738.169085999998</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.45">
@@ -8608,13 +8610,13 @@
         <v>32</v>
       </c>
       <c r="C18">
-        <v>766.51370999999995</v>
+        <v>23153.458517999999</v>
       </c>
       <c r="D18">
-        <v>517.47326499999997</v>
+        <v>16320.735236</v>
       </c>
       <c r="E18">
-        <v>773.47422800000004</v>
+        <v>24001.121573</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.45">
@@ -8622,13 +8624,13 @@
         <v>64</v>
       </c>
       <c r="C19">
-        <v>371.91076600000002</v>
+        <v>22764.920905000003</v>
       </c>
       <c r="D19">
-        <v>256.23837800000001</v>
+        <v>16129.511279999999</v>
       </c>
       <c r="E19">
-        <v>395.77799499999998</v>
+        <v>24267.876910999999</v>
       </c>
     </row>
   </sheetData>
@@ -8642,7 +8644,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X35" sqref="X35"/>
+      <selection activeCell="Z36" sqref="Z36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8680,13 +8682,13 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>919.62301300000001</v>
+        <v>1842.328088</v>
       </c>
       <c r="D2">
-        <v>179.101314</v>
+        <v>336.98767900000001</v>
       </c>
       <c r="E2">
-        <v>696.66354899999999</v>
+        <v>1338.4766599999998</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -8694,13 +8696,13 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>417.60313600000001</v>
+        <v>1630.8040209999999</v>
       </c>
       <c r="D3">
-        <v>156.03995900000001</v>
+        <v>1289.4868859999999</v>
       </c>
       <c r="E3">
-        <v>585.83232200000009</v>
+        <v>2214.1490180000001</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -8708,13 +8710,13 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>200.74024400000002</v>
+        <v>1657.2839739999999</v>
       </c>
       <c r="D4">
-        <v>116.41900199999999</v>
+        <v>913.99323800000002</v>
       </c>
       <c r="E4">
-        <v>535.49387899999999</v>
+        <v>3685.9497850000002</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -8722,13 +8724,13 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>99.146281000000002</v>
+        <v>1587.382398</v>
       </c>
       <c r="D5">
-        <v>88.838847999999999</v>
+        <v>1391.7510339999999</v>
       </c>
       <c r="E5">
-        <v>338.45861099999996</v>
+        <v>6352.0652230000005</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -8736,13 +8738,13 @@
         <v>32</v>
       </c>
       <c r="C6">
-        <v>48.621006000000001</v>
+        <v>1557.1203330000001</v>
       </c>
       <c r="D6">
-        <v>19.236562000000003</v>
+        <v>654.48222699999997</v>
       </c>
       <c r="E6">
-        <v>218.7397</v>
+        <v>6953.0150679999997</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -8750,13 +8752,13 @@
         <v>64</v>
       </c>
       <c r="C7">
-        <v>24.334616</v>
+        <v>1568.475103</v>
       </c>
       <c r="D7">
-        <v>12.412404</v>
+        <v>824.597082</v>
       </c>
       <c r="E7">
-        <v>113.20912799999999</v>
+        <v>8305.270579</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -8767,13 +8769,13 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>1574.480401</v>
+        <v>3143.5526620000001</v>
       </c>
       <c r="D8">
-        <v>273.08965500000005</v>
+        <v>516.59814600000004</v>
       </c>
       <c r="E8">
-        <v>1196.398173</v>
+        <v>2345.0947659999997</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -8781,13 +8783,13 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>705.70083900000009</v>
+        <v>2792.2023709999999</v>
       </c>
       <c r="D9">
-        <v>246.65773300000001</v>
+        <v>938.75314700000001</v>
       </c>
       <c r="E9">
-        <v>738.58021900000006</v>
+        <v>3015.3703369999998</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -8795,13 +8797,13 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>279.65802000000002</v>
+        <v>2534.4221979999998</v>
       </c>
       <c r="D10">
-        <v>188.79276999999999</v>
+        <v>1378.6770940000001</v>
       </c>
       <c r="E10">
-        <v>648.26373999999998</v>
+        <v>5437.6859489999997</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
@@ -8809,13 +8811,13 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <v>164.550059</v>
+        <v>2679.5521589999998</v>
       </c>
       <c r="D11">
-        <v>140.353972</v>
+        <v>2314.187336</v>
       </c>
       <c r="E11">
-        <v>424.941509</v>
+        <v>7199.2589280000002</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -8823,13 +8825,13 @@
         <v>32</v>
       </c>
       <c r="C12">
-        <v>81.694020000000009</v>
+        <v>2646.4874009999999</v>
       </c>
       <c r="D12">
-        <v>32.471094999999998</v>
+        <v>1091.683689</v>
       </c>
       <c r="E12">
-        <v>214.538827</v>
+        <v>6590.7346710000002</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -8837,13 +8839,13 @@
         <v>64</v>
       </c>
       <c r="C13">
-        <v>40.356572999999997</v>
+        <v>2602.847863</v>
       </c>
       <c r="D13">
-        <v>20.931922999999998</v>
+        <v>1419.085041</v>
       </c>
       <c r="E13">
-        <v>108.432823</v>
+        <v>6351.2031569999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -8854,13 +8856,13 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>1799.0464119999999</v>
+        <v>3625.124945</v>
       </c>
       <c r="D14">
-        <v>356.02531699999997</v>
+        <v>697.07932600000004</v>
       </c>
       <c r="E14">
-        <v>1969.667256</v>
+        <v>5328.0488609999993</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -8868,13 +8870,13 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>771.92786100000001</v>
+        <v>3370.6834079999999</v>
       </c>
       <c r="D15">
-        <v>298.03088600000001</v>
+        <v>1434.622519</v>
       </c>
       <c r="E15">
-        <v>1631.2498999999998</v>
+        <v>8573.2238010000001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -8882,13 +8884,13 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>365.542778</v>
+        <v>2945.1253860000002</v>
       </c>
       <c r="D16">
-        <v>260.77903400000002</v>
+        <v>1912.528129</v>
       </c>
       <c r="E16">
-        <v>1878.9681029999999</v>
+        <v>9069.4713530000008</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.45">
@@ -8896,13 +8898,13 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>199.91519699999998</v>
+        <v>3198.058125</v>
       </c>
       <c r="D17">
-        <v>42.761234999999999</v>
+        <v>945.72881900000004</v>
       </c>
       <c r="E17">
-        <v>945.63276300000007</v>
+        <v>17577.511300999999</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.45">
@@ -8910,13 +8912,13 @@
         <v>32</v>
       </c>
       <c r="C18">
-        <v>93.528789999999987</v>
+        <v>3102.866888</v>
       </c>
       <c r="D18">
-        <v>23.887888</v>
+        <v>826.375765</v>
       </c>
       <c r="E18">
-        <v>439.91199900000004</v>
+        <v>15351.100666999999</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.45">
@@ -8924,17 +8926,557 @@
         <v>64</v>
       </c>
       <c r="C19">
-        <v>46.391167000000003</v>
+        <v>2957.5107239999998</v>
       </c>
       <c r="D19">
-        <v>13.647536000000001</v>
+        <v>946.37794299999996</v>
       </c>
       <c r="E19">
-        <v>228.96158499999999</v>
+        <v>15542.536341000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B1BAA4-7808-4290-8CE8-6309C9156685}">
+  <dimension ref="A2:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="26.86328125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="20.796875" customWidth="1"/>
+    <col min="5" max="5" width="9.06640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>31361158.050999999</v>
+      </c>
+      <c r="C2">
+        <v>7919324.659</v>
+      </c>
+      <c r="D2">
+        <v>15770135.168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>21793743.456</v>
+      </c>
+      <c r="C3">
+        <v>7164208.8810000001</v>
+      </c>
+      <c r="D3">
+        <v>12107079.559</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>18201669.559</v>
+      </c>
+      <c r="C4">
+        <v>5689135.8130000001</v>
+      </c>
+      <c r="D4">
+        <v>10021444.551999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>18395182.688999999</v>
+      </c>
+      <c r="C5">
+        <v>17202302.087000001</v>
+      </c>
+      <c r="D5">
+        <v>14937551.918</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>18223721.625999998</v>
+      </c>
+      <c r="C6">
+        <v>15475009.431</v>
+      </c>
+      <c r="D6">
+        <v>13420573.001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>19026033.730999999</v>
+      </c>
+      <c r="C7">
+        <v>14408001.976</v>
+      </c>
+      <c r="D7">
+        <v>13786350.07</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>51409919.655000001</v>
+      </c>
+      <c r="C8">
+        <v>12869437.149</v>
+      </c>
+      <c r="D8">
+        <v>14702205.522</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>39009161.001000002</v>
+      </c>
+      <c r="C9">
+        <v>8415347.7679999992</v>
+      </c>
+      <c r="D9">
+        <v>9982409.4800000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>22195226.044</v>
+      </c>
+      <c r="C10">
+        <v>7642031.2230000002</v>
+      </c>
+      <c r="D10">
+        <v>9433640.7829999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>21458390.769000001</v>
+      </c>
+      <c r="C11">
+        <v>16479643.085000001</v>
+      </c>
+      <c r="D11">
+        <v>18330801.868000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <v>20856703.844999999</v>
+      </c>
+      <c r="C12">
+        <v>15977169.236</v>
+      </c>
+      <c r="D12">
+        <v>17023712.98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>64</v>
+      </c>
+      <c r="B13">
+        <v>20898758.035</v>
+      </c>
+      <c r="C13">
+        <v>15971148.16</v>
+      </c>
+      <c r="D13">
+        <v>17170486.681000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>35605599.368000001</v>
+      </c>
+      <c r="C14">
+        <v>28544136.761999998</v>
+      </c>
+      <c r="D14">
+        <v>15693545.309</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>29850519.802000001</v>
+      </c>
+      <c r="C15">
+        <v>19841074.765000001</v>
+      </c>
+      <c r="D15">
+        <v>8916372.5490000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>22840501.103999998</v>
+      </c>
+      <c r="C16">
+        <v>13525235.441</v>
+      </c>
+      <c r="D16">
+        <v>8550954.2799999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>23151701.236000001</v>
+      </c>
+      <c r="C17">
+        <v>15802498.16</v>
+      </c>
+      <c r="D17">
+        <v>24738169.085999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>23153458.517999999</v>
+      </c>
+      <c r="C18">
+        <v>16320735.236</v>
+      </c>
+      <c r="D18">
+        <v>24001121.572999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>64</v>
+      </c>
+      <c r="B19">
+        <v>22764920.905000001</v>
+      </c>
+      <c r="C19">
+        <v>16129511.279999999</v>
+      </c>
+      <c r="D19">
+        <v>24267876.910999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EAE7BF-14D4-470A-9D6A-9DBBAA260B29}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>2</v>
+      </c>
+      <c r="B1">
+        <v>1842328.088</v>
+      </c>
+      <c r="C1">
+        <v>336987.679</v>
+      </c>
+      <c r="D1">
+        <v>1338476.6599999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1630804.0209999999</v>
+      </c>
+      <c r="C2">
+        <v>1289486.8859999999</v>
+      </c>
+      <c r="D2">
+        <v>2214149.0180000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1657283.9739999999</v>
+      </c>
+      <c r="C3">
+        <v>913993.23800000001</v>
+      </c>
+      <c r="D3">
+        <v>3685949.7850000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>1587382.398</v>
+      </c>
+      <c r="C4">
+        <v>1391751.034</v>
+      </c>
+      <c r="D4">
+        <v>6352065.2230000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>1557120.3330000001</v>
+      </c>
+      <c r="C5">
+        <v>654482.22699999996</v>
+      </c>
+      <c r="D5">
+        <v>6953015.068</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>64</v>
+      </c>
+      <c r="B6">
+        <v>1568475.1029999999</v>
+      </c>
+      <c r="C6">
+        <v>824597.08200000005</v>
+      </c>
+      <c r="D6">
+        <v>8305270.5789999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>3143552.662</v>
+      </c>
+      <c r="C7">
+        <v>516598.14600000001</v>
+      </c>
+      <c r="D7">
+        <v>2345094.7659999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>2792202.3709999998</v>
+      </c>
+      <c r="C8">
+        <v>938753.147</v>
+      </c>
+      <c r="D8">
+        <v>3015370.3369999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2534422.1979999999</v>
+      </c>
+      <c r="C9">
+        <v>1378677.094</v>
+      </c>
+      <c r="D9">
+        <v>5437685.949</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>2679552.159</v>
+      </c>
+      <c r="C10">
+        <v>2314187.3360000001</v>
+      </c>
+      <c r="D10">
+        <v>7199258.9280000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>2646487.4010000001</v>
+      </c>
+      <c r="C11">
+        <v>1091683.689</v>
+      </c>
+      <c r="D11">
+        <v>6590734.6710000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>64</v>
+      </c>
+      <c r="B12">
+        <v>2602847.8629999999</v>
+      </c>
+      <c r="C12">
+        <v>1419085.041</v>
+      </c>
+      <c r="D12">
+        <v>6351203.1569999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>3625124.9449999998</v>
+      </c>
+      <c r="C13">
+        <v>697079.326</v>
+      </c>
+      <c r="D13">
+        <v>5328048.8609999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>3370683.4079999998</v>
+      </c>
+      <c r="C14">
+        <v>1434622.5190000001</v>
+      </c>
+      <c r="D14">
+        <v>8573223.8010000009</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>2945125.3859999999</v>
+      </c>
+      <c r="C15">
+        <v>1912528.129</v>
+      </c>
+      <c r="D15">
+        <v>9069471.3530000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>3198058.125</v>
+      </c>
+      <c r="C16">
+        <v>945728.81900000002</v>
+      </c>
+      <c r="D16">
+        <v>17577511.300999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>3102866.8879999998</v>
+      </c>
+      <c r="C17">
+        <v>826375.76500000001</v>
+      </c>
+      <c r="D17">
+        <v>15351100.666999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>64</v>
+      </c>
+      <c r="B18">
+        <v>2957510.7239999999</v>
+      </c>
+      <c r="C18">
+        <v>946377.94299999997</v>
+      </c>
+      <c r="D18">
+        <v>15542536.341</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>